<commit_message>
Update Intervention content and delivery.xlsx
Update to Intervention content and delivery spreadsheet
</commit_message>
<xml_diff>
--- a/Intervention content and delivery/Intervention content and delivery.xlsx
+++ b/Intervention content and delivery/Intervention content and delivery.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtpms_ucl_ac_uk/Documents/Galenos Project/Github preparation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtpms_ucl_ac_uk/Documents/Documents/GitHub/mental-health-ontology/Intervention content and delivery/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_D295A90A2C535A10C2167341E065F5EB470CA969" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81281C25-D131-477A-8C6D-B15E90249168}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_D295A90A2C535A10C2167341E065F5EB470CA969" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7059E1B0-F84A-4BA5-9220-7F4B5ACE94A3}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-15" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -301,13 +301,19 @@
   <si>
     <t>external parent class needs to be represented on Github spreadsheet for external entities
 Link to BCIO</t>
+  </si>
+  <si>
+    <t>Proposed</t>
+  </si>
+  <si>
+    <t>PS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,19 +334,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -415,14 +421,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -783,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -882,7 +948,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -912,13 +978,17 @@
       <c r="Q2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="10"/>
+      <c r="S2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T2" s="10"/>
+      <c r="U2" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
+      <c r="V2" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="3" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -951,10 +1021,14 @@
         <v>22</v>
       </c>
       <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
+      <c r="S3" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
+      <c r="V3" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="4" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -987,12 +1061,16 @@
         <v>22</v>
       </c>
       <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
+      <c r="S4" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-    </row>
-    <row r="5" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -1022,13 +1100,17 @@
       <c r="Q5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="10"/>
+      <c r="S5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T5" s="10"/>
+      <c r="U5" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
+      <c r="V5" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1060,11 +1142,15 @@
       <c r="Q6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="11"/>
-      <c r="S6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1097,10 +1183,14 @@
         <v>22</v>
       </c>
       <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
+      <c r="S7" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
+      <c r="V7" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -1133,10 +1223,14 @@
         <v>22</v>
       </c>
       <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
+      <c r="S8" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
+      <c r="V8" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -1169,10 +1263,14 @@
         <v>22</v>
       </c>
       <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
+      <c r="S9" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
+      <c r="V9" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1205,10 +1303,14 @@
         <v>22</v>
       </c>
       <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
+      <c r="S10" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
+      <c r="V10" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:22" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -1241,10 +1343,14 @@
         <v>22</v>
       </c>
       <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
+      <c r="S11" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
+      <c r="V11" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -1277,10 +1383,14 @@
         <v>22</v>
       </c>
       <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
+      <c r="S12" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
+      <c r="V12" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -1313,12 +1423,16 @@
         <v>22</v>
       </c>
       <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
+      <c r="S13" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-    </row>
-    <row r="14" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V13" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="7" t="s">
         <v>68</v>
@@ -1346,15 +1460,19 @@
       <c r="Q14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="R14" s="10"/>
+      <c r="S14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T14" s="10"/>
+      <c r="U14" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-    </row>
-    <row r="15" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V14" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="7" t="s">
         <v>59</v>
@@ -1382,15 +1500,19 @@
       <c r="Q15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="11" t="s">
+      <c r="R15" s="10"/>
+      <c r="S15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T15" s="10"/>
+      <c r="U15" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-    </row>
-    <row r="16" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V15" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="7" t="s">
         <v>62</v>
@@ -1418,15 +1540,19 @@
       <c r="Q16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="R16" s="10"/>
+      <c r="S16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T16" s="10"/>
+      <c r="U16" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-    </row>
-    <row r="17" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V16" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="7" t="s">
         <v>65</v>
@@ -1454,15 +1580,19 @@
       <c r="Q17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="11" t="s">
+      <c r="R17" s="10"/>
+      <c r="S17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T17" s="10"/>
+      <c r="U17" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-    </row>
-    <row r="18" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V17" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="7" t="s">
         <v>71</v>
@@ -1490,15 +1620,19 @@
       <c r="Q18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R18" s="11" t="s">
+      <c r="R18" s="10"/>
+      <c r="S18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T18" s="10"/>
+      <c r="U18" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-    </row>
-    <row r="19" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V18" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="7" t="s">
         <v>74</v>
@@ -1526,15 +1660,19 @@
       <c r="Q19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="11" t="s">
+      <c r="R19" s="10"/>
+      <c r="S19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T19" s="10"/>
+      <c r="U19" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-    </row>
-    <row r="20" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V19" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="10"/>
       <c r="B20" s="7" t="s">
         <v>77</v>
@@ -1562,15 +1700,19 @@
       <c r="Q20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R20" s="11" t="s">
+      <c r="R20" s="10"/>
+      <c r="S20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T20" s="10"/>
+      <c r="U20" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-    </row>
-    <row r="21" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="V20" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="7" t="s">
         <v>79</v>
@@ -1598,15 +1740,19 @@
       <c r="Q21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R21" s="11" t="s">
+      <c r="R21" s="10"/>
+      <c r="S21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T21" s="10"/>
+      <c r="U21" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10"/>
-    </row>
-    <row r="22" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="V21" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="116" x14ac:dyDescent="0.35">
       <c r="A22" s="10"/>
       <c r="B22" s="13" t="s">
         <v>85</v>
@@ -1634,33 +1780,20 @@
       <c r="Q22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R22" s="11" t="s">
+      <c r="R22" s="10"/>
+      <c r="S22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T22" s="10"/>
+      <c r="U22" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
+      <c r="V22" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B5:B13">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B17">
-    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D13">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>